<commit_message>
data build and updatae
</commit_message>
<xml_diff>
--- a/build/input/KoreaAsiaHFtrade.xlsx
+++ b/build/input/KoreaAsiaHFtrade.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hj/Documents/GitHub/JapanKoreaTradeConflict/build/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FFD18F8-15A2-8048-9E66-2FBF391030B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC3216-9506-ED49-8CC2-2BB86216E27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-3720" windowWidth="25600" windowHeight="26560"/>
+    <workbookView xWindow="-25600" yWindow="-3720" windowWidth="25600" windowHeight="26560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KoreaNorthAmericaHFtrade" sheetId="1" r:id="rId1"/>
@@ -112,8 +112,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,12 +272,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF363636"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -711,20 +705,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1081,11 +1072,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1117,510 +1108,490 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1">
-        <v>2021</v>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
         <v>2811111000</v>
       </c>
-      <c r="C2" s="3">
-        <v>7046252</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2446464.98</v>
-      </c>
-      <c r="E2" s="3">
-        <v>41385736</v>
-      </c>
-      <c r="F2" s="4">
-        <v>24053192.789999999</v>
+      <c r="C2" s="2">
+        <v>12571247</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4321074.5999999996</v>
+      </c>
+      <c r="E2" s="2">
+        <v>71817627</v>
+      </c>
+      <c r="F2" s="3">
+        <v>42200869.640000001</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B3">
         <v>2811111000</v>
       </c>
-      <c r="C3" s="3">
-        <v>12571247</v>
-      </c>
-      <c r="D3" s="4">
-        <v>4321074.5999999996</v>
-      </c>
-      <c r="E3" s="3">
-        <v>71817627</v>
-      </c>
-      <c r="F3" s="4">
-        <v>42200869.640000001</v>
+      <c r="C3" s="2">
+        <v>12622866</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4199282.75</v>
+      </c>
+      <c r="E3" s="2">
+        <v>111664329</v>
+      </c>
+      <c r="F3" s="3">
+        <v>60353161.600000001</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B4">
         <v>2811111000</v>
       </c>
-      <c r="C4" s="3">
-        <v>12622866</v>
-      </c>
-      <c r="D4" s="4">
-        <v>4199282.75</v>
-      </c>
-      <c r="E4" s="3">
-        <v>111664329</v>
-      </c>
-      <c r="F4" s="4">
-        <v>60353161.600000001</v>
+      <c r="C4" s="2">
+        <v>11700604</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4056211.2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>158962152</v>
+      </c>
+      <c r="F4" s="3">
+        <v>83299206.930000007</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2811111000</v>
       </c>
-      <c r="C5" s="3">
-        <v>11700604</v>
-      </c>
-      <c r="D5" s="4">
-        <v>4056211.2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>158962152</v>
-      </c>
-      <c r="F5" s="4">
-        <v>83299206.930000007</v>
+      <c r="C5" s="2">
+        <v>10507690</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3514693.16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>91252408</v>
+      </c>
+      <c r="F5" s="3">
+        <v>64729167.75</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2811111000</v>
       </c>
-      <c r="C6" s="3">
-        <v>10507690</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3514693.16</v>
-      </c>
-      <c r="E6" s="3">
-        <v>91252408</v>
-      </c>
-      <c r="F6" s="4">
-        <v>64729167.75</v>
+      <c r="C6" s="2">
+        <v>9691807</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3284678</v>
+      </c>
+      <c r="E6" s="2">
+        <v>68346688</v>
+      </c>
+      <c r="F6" s="3">
+        <v>52582679.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B7">
         <v>2811111000</v>
       </c>
-      <c r="C7" s="3">
-        <v>9691807</v>
+      <c r="C7" s="2">
+        <v>6606064</v>
       </c>
       <c r="D7" s="3">
-        <v>3284678</v>
-      </c>
-      <c r="E7" s="3">
-        <v>68346688</v>
-      </c>
-      <c r="F7" s="4">
-        <v>52582679.5</v>
+        <v>2438392.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>74183637</v>
+      </c>
+      <c r="F7" s="2">
+        <v>58001045</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2811111000</v>
       </c>
-      <c r="C8" s="3">
-        <v>6606064</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2438392.6</v>
-      </c>
-      <c r="E8" s="3">
-        <v>74183637</v>
-      </c>
-      <c r="F8" s="3">
-        <v>58001045</v>
+      <c r="C8" s="2">
+        <v>3781350</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1549769.9</v>
+      </c>
+      <c r="E8" s="2">
+        <v>78854764</v>
+      </c>
+      <c r="F8" s="2">
+        <v>55351770</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
+      <c r="A9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B9">
         <v>2811111000</v>
       </c>
-      <c r="C9" s="3">
-        <v>3781350</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1549769.9</v>
-      </c>
-      <c r="E9" s="3">
-        <v>78854764</v>
-      </c>
-      <c r="F9" s="3">
-        <v>55351770</v>
+      <c r="C9" s="2">
+        <v>1712118</v>
+      </c>
+      <c r="D9" s="3">
+        <v>745942.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>65117762</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42117436</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
+      <c r="A10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B10">
         <v>2811111000</v>
       </c>
-      <c r="C10" s="3">
-        <v>1712118</v>
-      </c>
-      <c r="D10" s="4">
-        <v>745942.5</v>
-      </c>
-      <c r="E10" s="3">
-        <v>65117762</v>
-      </c>
-      <c r="F10" s="3">
-        <v>42117436</v>
+      <c r="C10" s="2">
+        <v>1373450</v>
+      </c>
+      <c r="D10" s="3">
+        <v>598524.4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>70680766</v>
+      </c>
+      <c r="F10" s="2">
+        <v>36126685</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B11">
         <v>2811111000</v>
       </c>
-      <c r="C11" s="3">
-        <v>1373450</v>
-      </c>
-      <c r="D11" s="4">
-        <v>598524.4</v>
-      </c>
-      <c r="E11" s="3">
-        <v>70680766</v>
-      </c>
-      <c r="F11" s="3">
-        <v>36126685</v>
+      <c r="C11" s="2">
+        <v>1682204</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1265785.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>67123332</v>
+      </c>
+      <c r="F11" s="2">
+        <v>30822866</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
+      <c r="A12" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B12">
         <v>2811111000</v>
       </c>
-      <c r="C12" s="3">
-        <v>1682204</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1265785.5</v>
-      </c>
-      <c r="E12" s="3">
-        <v>67123332</v>
-      </c>
-      <c r="F12" s="3">
-        <v>30822866</v>
+      <c r="C12" s="2">
+        <v>1950829</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1702141.5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>41212482</v>
+      </c>
+      <c r="F12" s="2">
+        <v>23245782</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
+      <c r="A13" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B13">
         <v>2811111000</v>
       </c>
-      <c r="C13" s="3">
-        <v>1950829</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1702141.5</v>
-      </c>
-      <c r="E13" s="3">
-        <v>41212482</v>
-      </c>
-      <c r="F13" s="3">
-        <v>23245782</v>
+      <c r="C13" s="2">
+        <v>770354</v>
+      </c>
+      <c r="D13" s="2">
+        <v>611341</v>
+      </c>
+      <c r="E13" s="2">
+        <v>28551874</v>
+      </c>
+      <c r="F13" s="2">
+        <v>17383943</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
+      <c r="A14" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B14">
         <v>2811111000</v>
       </c>
-      <c r="C14" s="3">
-        <v>770354</v>
-      </c>
-      <c r="D14" s="3">
-        <v>611341</v>
-      </c>
-      <c r="E14" s="3">
-        <v>28551874</v>
-      </c>
-      <c r="F14" s="3">
-        <v>17383943</v>
+      <c r="C14" s="2">
+        <v>1294948</v>
+      </c>
+      <c r="D14" s="2">
+        <v>668237</v>
+      </c>
+      <c r="E14" s="2">
+        <v>33503393</v>
+      </c>
+      <c r="F14" s="2">
+        <v>21020449</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
+      <c r="A15" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B15">
         <v>2811111000</v>
       </c>
-      <c r="C15" s="3">
-        <v>1294948</v>
+      <c r="C15" s="2">
+        <v>1666475</v>
       </c>
       <c r="D15" s="3">
-        <v>668237</v>
-      </c>
-      <c r="E15" s="3">
-        <v>33503393</v>
-      </c>
-      <c r="F15" s="3">
-        <v>21020449</v>
+        <v>679603.7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>21275272</v>
+      </c>
+      <c r="F15" s="2">
+        <v>17672104</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
+      <c r="A16" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B16">
         <v>2811111000</v>
       </c>
-      <c r="C16" s="3">
-        <v>1666475</v>
-      </c>
-      <c r="D16" s="4">
-        <v>679603.7</v>
-      </c>
-      <c r="E16" s="3">
-        <v>21275272</v>
-      </c>
-      <c r="F16" s="3">
-        <v>17672104</v>
+      <c r="C16" s="2">
+        <v>783481</v>
+      </c>
+      <c r="D16" s="2">
+        <v>391065</v>
+      </c>
+      <c r="E16" s="2">
+        <v>14920669</v>
+      </c>
+      <c r="F16" s="2">
+        <v>12239156</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
+      <c r="A17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B17">
         <v>2811111000</v>
       </c>
-      <c r="C17" s="3">
-        <v>783481</v>
-      </c>
-      <c r="D17" s="3">
-        <v>391065</v>
-      </c>
-      <c r="E17" s="3">
-        <v>14920669</v>
-      </c>
-      <c r="F17" s="3">
-        <v>12239156</v>
+      <c r="C17" s="2">
+        <v>530551</v>
+      </c>
+      <c r="D17" s="2">
+        <v>72976</v>
+      </c>
+      <c r="E17" s="2">
+        <v>13451487</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9161376</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
+      <c r="A18" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B18">
         <v>2811111000</v>
       </c>
-      <c r="C18" s="3">
-        <v>530551</v>
+      <c r="C18" s="2">
+        <v>944670</v>
       </c>
       <c r="D18" s="3">
-        <v>72976</v>
-      </c>
-      <c r="E18" s="3">
-        <v>13451487</v>
-      </c>
-      <c r="F18" s="3">
-        <v>9161376</v>
+        <v>121551.5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>10779514</v>
+      </c>
+      <c r="F18" s="2">
+        <v>7280345</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
+      <c r="A19" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B19">
         <v>2811111000</v>
       </c>
-      <c r="C19" s="3">
-        <v>944670</v>
-      </c>
-      <c r="D19" s="4">
-        <v>121551.5</v>
-      </c>
-      <c r="E19" s="3">
-        <v>10779514</v>
-      </c>
-      <c r="F19" s="3">
-        <v>7280345</v>
+      <c r="C19" s="2">
+        <v>438541</v>
+      </c>
+      <c r="D19" s="3">
+        <v>69902.399999999994</v>
+      </c>
+      <c r="E19" s="2">
+        <v>7825648</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5409870</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
+      <c r="A20" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B20">
         <v>2811111000</v>
       </c>
-      <c r="C20" s="3">
-        <v>438541</v>
-      </c>
-      <c r="D20" s="4">
-        <v>69902.399999999994</v>
-      </c>
-      <c r="E20" s="3">
-        <v>7825648</v>
-      </c>
-      <c r="F20" s="3">
-        <v>5409870</v>
+      <c r="C20" s="2">
+        <v>45782</v>
+      </c>
+      <c r="D20" s="2">
+        <v>17680</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5923117</v>
+      </c>
+      <c r="F20" s="2">
+        <v>4227135</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
+      <c r="A21" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B21">
         <v>2811111000</v>
       </c>
-      <c r="C21" s="3">
-        <v>45782</v>
-      </c>
-      <c r="D21" s="3">
-        <v>17680</v>
-      </c>
-      <c r="E21" s="3">
-        <v>5923117</v>
-      </c>
-      <c r="F21" s="3">
-        <v>4227135</v>
+      <c r="C21" s="2">
+        <v>1989</v>
+      </c>
+      <c r="D21" s="1">
+        <v>752</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6254750</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4090445</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
+      <c r="A22" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B22">
         <v>2811111000</v>
       </c>
-      <c r="C22" s="3">
-        <v>1989</v>
-      </c>
-      <c r="D22" s="2">
-        <v>752</v>
-      </c>
-      <c r="E22" s="3">
-        <v>6254750</v>
-      </c>
-      <c r="F22" s="3">
-        <v>4090445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23">
-        <v>2811111000</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="C22" s="1">
         <v>0</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E22" s="2">
         <v>6533764</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F22" s="2">
         <v>3758850</v>
       </c>
     </row>
+    <row r="28" spans="1:6">
+      <c r="B28" s="1"/>
+    </row>
     <row r="29" spans="1:6">
-      <c r="B29" s="2"/>
+      <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" s="2"/>
+      <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" s="2"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="2"/>
+      <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="2"/>
+      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="2"/>
+      <c r="B34" s="1"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="2"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="2"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="2"/>
+      <c r="B37" s="1"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="2"/>
+      <c r="B38" s="1"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="2"/>
+      <c r="B39" s="1"/>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="2"/>
+      <c r="B40" s="1"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="2"/>
+      <c r="B41" s="1"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="2"/>
+      <c r="B42" s="1"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="2"/>
+      <c r="B43" s="1"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="2"/>
+      <c r="B44" s="1"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="2"/>
+      <c r="B45" s="1"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="2"/>
+      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="2"/>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="2"/>
+      <c r="B48" s="1"/>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="2"/>
+      <c r="B49" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>